<commit_message>
fix wrong input data
</commit_message>
<xml_diff>
--- a/Input_values.xlsx
+++ b/Input_values.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikitabelyak/Dropbox (Aalto)/TSEP/Nordic_case_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157FA683-6FA8-674A-8905-E9ACEC60EEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F669A57C-A1D5-F44D-B583-0D8C5AA85863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="16840" xr2:uid="{C762C8DE-9A4E-C342-80CA-38E28E725733}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22340" xr2:uid="{C762C8DE-9A4E-C342-80CA-38E28E725733}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">TRANSMISSION EXPANSION BUDGET </t>
   </si>
   <si>
-    <t xml:space="preserve">GENERATION EXPANSION BUDGET </t>
-  </si>
-  <si>
     <t>SMALL</t>
   </si>
   <si>
@@ -89,14 +86,18 @@
   </si>
   <si>
     <t>EUR/T</t>
+  </si>
+  <si>
+    <t>GENERATION EXPANSION BUDGET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;"/>
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -144,14 +145,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,7 +172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -458,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,102 +468,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A8B318-8742-3F49-973D-1B0DF04810E9}">
-  <dimension ref="B1:AB11"/>
+  <dimension ref="B1:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="2"/>
+      <c r="O1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="2"/>
-      <c r="O1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
     </row>
     <row r="2" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B3" s="7">
-        <f xml:space="preserve"> 60000000 / 52</f>
-        <v>1153846.1538461538</v>
-      </c>
-      <c r="D3" s="7">
-        <f xml:space="preserve"> 3000000000/52</f>
-        <v>57692307.692307696</v>
-      </c>
-      <c r="F3" s="7">
-        <f>60000000/52</f>
-        <v>1153846.1538461538</v>
-      </c>
-      <c r="H3" s="7">
-        <f>3000000000/52</f>
-        <v>57692307.692307696</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="B3" s="5">
+        <f xml:space="preserve"> 25000000000/10/4/365</f>
+        <v>1712328.7671232878</v>
+      </c>
+      <c r="D3" s="5">
+        <f>B3*2</f>
+        <v>3424657.5342465756</v>
+      </c>
+      <c r="F3" s="5">
+        <f>3000000000/365</f>
+        <v>8219178.0821917811</v>
+      </c>
+      <c r="H3" s="5">
+        <f>F3*2</f>
+        <v>16438356.164383562</v>
+      </c>
+      <c r="J3" s="4">
         <v>0.05</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="4">
         <v>0.2</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="4"/>
       <c r="N3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -597,142 +600,154 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="R4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="7"/>
+      <c r="U4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="7"/>
+      <c r="X4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="R4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="S4" s="5"/>
-      <c r="U4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V4" s="5"/>
-      <c r="X4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y4" s="5"/>
-      <c r="AA4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB4" s="5"/>
+      <c r="Y4" s="7"/>
+      <c r="AA4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB4" s="7"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="N5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T5" s="3"/>
       <c r="U5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.2">
       <c r="N6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="7">
+        <v>12</v>
+      </c>
+      <c r="O6" s="5">
         <f>ROUND(R11*O3,  0)</f>
         <v>0</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="5">
         <f>ROUND(R10*P3, 0)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="5">
         <f>ROUND($R$11*R3,0)</f>
         <v>8</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="5">
         <f>ROUND(R10*S3, 0)</f>
         <v>70</v>
       </c>
-      <c r="U6" s="7">
+      <c r="U6" s="5">
         <f>ROUND(R11*U3, 0)</f>
         <v>3</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="5">
         <f>ROUND(R10*V3, 0)</f>
         <v>25</v>
       </c>
-      <c r="X6" s="7">
+      <c r="X6" s="5">
         <f>ROUND(R11*X3, 0)</f>
         <v>4</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Y6" s="5">
         <f>ROUND(R10*Y3, 0)</f>
         <v>36</v>
       </c>
-      <c r="AA6" s="7">
+      <c r="AA6" s="5">
         <f>ROUND(R11*AA3, 0)</f>
         <v>2</v>
       </c>
-      <c r="AB6" s="7">
+      <c r="AB6" s="5">
         <f>ROUND(R10*AB3,0)</f>
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="Q10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R10">
         <v>71</v>
       </c>
       <c r="S10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="Q11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R11">
         <v>8</v>
       </c>
       <c r="S11" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="U4:V4"/>
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="O1:AB1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="O4:P4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>